<commit_message>
Update test data for Quick_Search and Simple_Search
</commit_message>
<xml_diff>
--- a/data/Func_QuickSearch.xlsx
+++ b/data/Func_QuickSearch.xlsx
@@ -24,13 +24,13 @@
     <t>MDCPOrgID</t>
   </si>
   <si>
-    <t>OPP-0002869474</t>
-  </si>
-  <si>
     <t>ProductNumber</t>
   </si>
   <si>
     <t>G1S77A</t>
+  </si>
+  <si>
+    <t>OPE-0003018780</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,18 +390,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>145152418</v>
+        <v>76846561</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>